<commit_message>
Benchmarking Complete: post words, get anagrams, delete words and get stats
</commit_message>
<xml_diff>
--- a/anagrams_rb/anagram_benchmarking.xlsx
+++ b/anagrams_rb/anagram_benchmarking.xlsx
@@ -8,13 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2d43b0a7edc15fe4/Documents/GitHub/anagramsAPI/anagrams_rb/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="C15D0559CDA1AA62CEC282FF417EA8F840AC62A6" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{6DB6CE5E-2101-46D7-AD73-5C43A4C8A941}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="C15D0559CDA1AA62CEC282FF417EA8F840AC62A6" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{7AB0185D-923E-4F7D-AAEB-89F11BF31F4D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="benchmark_post" sheetId="1" r:id="rId1"/>
+    <sheet name="benchmark_plots" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -593,13 +599,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Batch Posting </a:t>
+              <a:t>POST Words</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -713,10 +714,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>benchmark_post!$A$1:$A$16</c:f>
+              <c:f>[1]benchmark_post!$A$1:$A$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
@@ -752,75 +753,51 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>8000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>80000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>benchmark_post!$B$1:$B$16</c:f>
+              <c:f>[1]benchmark_post!$B$1:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.6021000000000001E-2</c:v>
+                  <c:v>1.8100000044796598E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0498000000000001E-2</c:v>
+                  <c:v>3.2948000007308999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5420000000000002E-2</c:v>
+                  <c:v>4.7286999993957503E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.6068000000000006E-2</c:v>
+                  <c:v>8.4992999967653304E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10431799999999999</c:v>
+                  <c:v>9.6575000032316893E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20813899999999999</c:v>
+                  <c:v>0.19954000000143399</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.39658399999999999</c:v>
+                  <c:v>0.37714399996912101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.81247599999999998</c:v>
+                  <c:v>0.811535999993793</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.97496700000000003</c:v>
+                  <c:v>1.0876430000062101</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.0001549999999999</c:v>
+                  <c:v>2.0856550000025802</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.0347619999999997</c:v>
+                  <c:v>4.1456800000160001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.7959009999999997</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9.8880379999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>19.903305</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>39.314788999999998</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>78.177730999999994</c:v>
+                  <c:v>7.9355390000273403</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1128,7 +1105,1703 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GET Aanagrams</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:noFill/>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.36550276781151592"/>
+                  <c:y val="0.15474914193418129"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[2]benchmark_get!$A$1:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[2]benchmark_get!$B$1:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.9157000011764401E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7626999972853803E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.112130000023171</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.24994199996581301</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30319700000109101</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.58184200001414799</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1534110000357001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.3734310000436301</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8222949999617399</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5782860000035699</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.3090580000425</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>22.789019000018001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1000-4D8B-93B4-008669095E10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="602979183"/>
+        <c:axId val="845456863"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="602979183"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> N</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="845456863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="845456863"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="602979183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>DELETE Words</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:noFill/>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.38586298707853828"/>
+                  <c:y val="0.20391762671611008"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[3]benchmark_delete!$A$1:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[3]benchmark_delete!$B$1:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>2.7047000010497799E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6663999983575195E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.127017999999225</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26417400001082503</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32737200002884398</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61586700001498595</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.25611900002695</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5693120000068999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.10164000000804</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.27218299999367</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.4969820000114</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.852335000003201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EF60-46FD-9014-8473C2E13A9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="602979183"/>
+        <c:axId val="845456863"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="602979183"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> N</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="845456863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="845456863"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Time</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="602979183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>GET Stats</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:noFill/>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[4]benchmark_stats!$A$1:$A$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[4]benchmark_stats!$B$1:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>5.5489999940618803E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6729999962262801E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.8929999833926498E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.3050000094808603E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.55200002761557E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.2949999808333797E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1530000055208802E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.0549999945797E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.9510000390000598E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9699999983422397E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.7410000008530897E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.2619999623857404E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-503B-4DAF-90D7-EBF050D5CA5E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="602979183"/>
+        <c:axId val="845456863"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="602979183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="10"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>N</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="845456863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="845456863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="602979183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1684,20 +3357,1568 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>419099</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1722,7 +4943,561 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>238124</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A48FA658-6F9E-4890-B890-09BE380F51AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>57151</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{824CA800-C035-4632-828F-E70F8D341D7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1363C384-703C-4899-AC4F-E1434432DAFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="benchmark_post"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1">
+            <v>10</v>
+          </cell>
+          <cell r="B1">
+            <v>1.8100000044796598E-2</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>20</v>
+          </cell>
+          <cell r="B2">
+            <v>3.2948000007308999E-2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>40</v>
+          </cell>
+          <cell r="B3">
+            <v>4.7286999993957503E-2</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>80</v>
+          </cell>
+          <cell r="B4">
+            <v>8.4992999967653304E-2</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>100</v>
+          </cell>
+          <cell r="B5">
+            <v>9.6575000032316893E-2</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>200</v>
+          </cell>
+          <cell r="B6">
+            <v>0.19954000000143399</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>400</v>
+          </cell>
+          <cell r="B7">
+            <v>0.37714399996912101</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>800</v>
+          </cell>
+          <cell r="B8">
+            <v>0.811535999993793</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>1000</v>
+          </cell>
+          <cell r="B9">
+            <v>1.0876430000062101</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>2000</v>
+          </cell>
+          <cell r="B10">
+            <v>2.0856550000025802</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>4000</v>
+          </cell>
+          <cell r="B11">
+            <v>4.1456800000160001</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>8000</v>
+          </cell>
+          <cell r="B12">
+            <v>7.9355390000273403</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="benchmark_get"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1">
+            <v>10</v>
+          </cell>
+          <cell r="B1">
+            <v>2.9157000011764401E-2</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>20</v>
+          </cell>
+          <cell r="B2">
+            <v>5.7626999972853803E-2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>40</v>
+          </cell>
+          <cell r="B3">
+            <v>0.112130000023171</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>80</v>
+          </cell>
+          <cell r="B4">
+            <v>0.24994199996581301</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>100</v>
+          </cell>
+          <cell r="B5">
+            <v>0.30319700000109101</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>200</v>
+          </cell>
+          <cell r="B6">
+            <v>0.58184200001414799</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>400</v>
+          </cell>
+          <cell r="B7">
+            <v>1.1534110000357001</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>800</v>
+          </cell>
+          <cell r="B8">
+            <v>2.3734310000436301</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>1000</v>
+          </cell>
+          <cell r="B9">
+            <v>2.8222949999617399</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>2000</v>
+          </cell>
+          <cell r="B10">
+            <v>5.5782860000035699</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>4000</v>
+          </cell>
+          <cell r="B11">
+            <v>11.3090580000425</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>8000</v>
+          </cell>
+          <cell r="B12">
+            <v>22.789019000018001</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="benchmark_delete"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1">
+            <v>10</v>
+          </cell>
+          <cell r="B1">
+            <v>2.7047000010497799E-2</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>20</v>
+          </cell>
+          <cell r="B2">
+            <v>6.6663999983575195E-2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>40</v>
+          </cell>
+          <cell r="B3">
+            <v>0.127017999999225</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>80</v>
+          </cell>
+          <cell r="B4">
+            <v>0.26417400001082503</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>100</v>
+          </cell>
+          <cell r="B5">
+            <v>0.32737200002884398</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>200</v>
+          </cell>
+          <cell r="B6">
+            <v>0.61586700001498595</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>400</v>
+          </cell>
+          <cell r="B7">
+            <v>1.25611900002695</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>800</v>
+          </cell>
+          <cell r="B8">
+            <v>2.5693120000068999</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>1000</v>
+          </cell>
+          <cell r="B9">
+            <v>3.10164000000804</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>2000</v>
+          </cell>
+          <cell r="B10">
+            <v>6.27218299999367</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>4000</v>
+          </cell>
+          <cell r="B11">
+            <v>12.4969820000114</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>8000</v>
+          </cell>
+          <cell r="B12">
+            <v>24.852335000003201</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="benchmark_stats"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1">
+            <v>10</v>
+          </cell>
+          <cell r="B1">
+            <v>5.5489999940618803E-3</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2">
+            <v>20</v>
+          </cell>
+          <cell r="B2">
+            <v>6.6729999962262801E-3</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3">
+            <v>40</v>
+          </cell>
+          <cell r="B3">
+            <v>6.8929999833926498E-3</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4">
+            <v>80</v>
+          </cell>
+          <cell r="B4">
+            <v>4.3050000094808603E-3</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5">
+            <v>100</v>
+          </cell>
+          <cell r="B5">
+            <v>4.55200002761557E-3</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6">
+            <v>200</v>
+          </cell>
+          <cell r="B6">
+            <v>5.2949999808333797E-3</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7">
+            <v>400</v>
+          </cell>
+          <cell r="B7">
+            <v>5.1530000055208802E-3</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8">
+            <v>800</v>
+          </cell>
+          <cell r="B8">
+            <v>7.0549999945797E-3</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9">
+            <v>1000</v>
+          </cell>
+          <cell r="B9">
+            <v>4.9510000390000598E-3</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10">
+            <v>2000</v>
+          </cell>
+          <cell r="B10">
+            <v>5.9699999983422397E-3</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11">
+            <v>4000</v>
+          </cell>
+          <cell r="B11">
+            <v>5.7410000008530897E-3</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12">
+            <v>8000</v>
+          </cell>
+          <cell r="B12">
+            <v>5.2619999623857404E-3</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2022,143 +5797,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>10</v>
-      </c>
-      <c r="B1">
-        <v>1.6021000000000001E-2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>20</v>
-      </c>
-      <c r="B2">
-        <v>3.0498000000000001E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>40</v>
-      </c>
-      <c r="B3">
-        <v>4.5420000000000002E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>80</v>
-      </c>
-      <c r="B4">
-        <v>8.6068000000000006E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>100</v>
-      </c>
-      <c r="B5">
-        <v>0.10431799999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>200</v>
-      </c>
-      <c r="B6">
-        <v>0.20813899999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>400</v>
-      </c>
-      <c r="B7">
-        <v>0.39658399999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>800</v>
-      </c>
-      <c r="B8">
-        <v>0.81247599999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1000</v>
-      </c>
-      <c r="B9">
-        <v>0.97496700000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2000</v>
-      </c>
-      <c r="B10">
-        <v>2.0001549999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>4000</v>
-      </c>
-      <c r="B11">
-        <v>4.0347619999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>8000</v>
-      </c>
-      <c r="B12">
-        <v>7.7959009999999997</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>10000</v>
-      </c>
-      <c r="B13">
-        <v>9.8880379999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>20000</v>
-      </c>
-      <c r="B14">
-        <v>19.903305</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>40000</v>
-      </c>
-      <c r="B15">
-        <v>39.314788999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>80000</v>
-      </c>
-      <c r="B16">
-        <v>78.177730999999994</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>